<commit_message>
Refactored to main Driver and ExcelParser class to parse out first sheet into list of data
</commit_message>
<xml_diff>
--- a/src/main/resources/Crypto Tracker.xlsx
+++ b/src/main/resources/Crypto Tracker.xlsx
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -137,9 +137,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -676,77 +673,59 @@
         <v>50.25826872</v>
       </c>
     </row>
-    <row r="20">
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="8"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="9"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="9"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="9"/>
-    </row>
     <row r="48">
-      <c r="B48" s="9"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49">
-      <c r="B49" s="9"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="55">
-      <c r="B55" s="9"/>
+      <c r="B55" s="8"/>
     </row>
     <row r="56">
-      <c r="B56" s="9"/>
+      <c r="B56" s="8"/>
     </row>
     <row r="62">
-      <c r="B62" s="9"/>
+      <c r="B62" s="8"/>
     </row>
     <row r="63">
-      <c r="B63" s="9"/>
+      <c r="B63" s="8"/>
     </row>
     <row r="69">
-      <c r="B69" s="9"/>
+      <c r="B69" s="8"/>
     </row>
     <row r="70">
-      <c r="B70" s="9"/>
+      <c r="B70" s="8"/>
     </row>
     <row r="76">
-      <c r="B76" s="9"/>
+      <c r="B76" s="8"/>
     </row>
     <row r="77">
-      <c r="B77" s="9"/>
+      <c r="B77" s="8"/>
     </row>
     <row r="83">
-      <c r="B83" s="9"/>
+      <c r="B83" s="8"/>
     </row>
     <row r="84">
-      <c r="B84" s="9"/>
+      <c r="B84" s="8"/>
     </row>
     <row r="90">
-      <c r="B90" s="9"/>
+      <c r="B90" s="8"/>
     </row>
     <row r="91">
-      <c r="B91" s="9"/>
+      <c r="B91" s="8"/>
     </row>
     <row r="97">
-      <c r="B97" s="9"/>
+      <c r="B97" s="8"/>
     </row>
     <row r="98">
-      <c r="B98" s="9"/>
+      <c r="B98" s="8"/>
     </row>
     <row r="104">
-      <c r="B104" s="9"/>
+      <c r="B104" s="8"/>
     </row>
     <row r="105">
-      <c r="B105" s="9"/>
+      <c r="B105" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -799,16 +778,16 @@
         <v>4513.1946</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D8" si="1">B3*C3</f>
+        <f t="shared" ref="D3:D9" si="1">B3*C3</f>
         <v>50.51167396</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIF(D3:D1000, "&gt;0")</f>
-        <v>200.584224</v>
+        <v>251.028024</v>
       </c>
       <c r="F3" s="5">
         <f>SUMPRODUCT(D3:D1000/E3, C3:C1000*(C3:C1000&gt;0))</f>
-        <v>4304.072497</v>
+        <v>4102.305254</v>
       </c>
     </row>
     <row r="4">
@@ -878,12 +857,27 @@
       <c r="B8" s="1">
         <v>0.023699</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>-4300.0</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="1"/>
         <v>-101.9057</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>44344.0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.015286</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3300.0</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="1"/>
+        <v>50.4438</v>
       </c>
     </row>
   </sheetData>
@@ -927,13 +921,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>44306.0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>41.63</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1.1364</v>
       </c>
       <c r="D3" s="5">
@@ -950,13 +944,13 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>44312.0</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>41.63</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>-1.16</v>
       </c>
       <c r="D4" s="5">
@@ -965,13 +959,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>44312.0</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>20.42</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>1.1711</v>
       </c>
       <c r="D5" s="5">
@@ -980,13 +974,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>44312.0</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>20.42</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>-1.18</v>
       </c>
       <c r="D6" s="5">

</xml_diff>

<commit_message>
Extended logic to include multiple sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/Crypto Tracker.xlsx
+++ b/src/main/resources/Crypto Tracker.xlsx
@@ -778,16 +778,16 @@
         <v>4513.1946</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D9" si="1">B3*C3</f>
+        <f t="shared" ref="D3:D10" si="1">B3*C3</f>
         <v>50.51167396</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIF(D3:D1000, "&gt;0")</f>
-        <v>251.028024</v>
+        <v>301.198274</v>
       </c>
       <c r="F3" s="5">
         <f>SUMPRODUCT(D3:D1000/E3, C3:C1000*(C3:C1000&gt;0))</f>
-        <v>4102.305254</v>
+        <v>3960.337749</v>
       </c>
     </row>
     <row r="4">
@@ -878,6 +878,21 @@
       <c r="D9" s="5">
         <f t="shared" si="1"/>
         <v>50.4438</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>44344.0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.015437</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3250.0</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="1"/>
+        <v>50.17025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed ExcelParser logic from using ArrayList to HashMap to associate coin name to coin transaction data
</commit_message>
<xml_diff>
--- a/src/main/resources/Crypto Tracker.xlsx
+++ b/src/main/resources/Crypto Tracker.xlsx
@@ -16,29 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Bitcoin</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>(BTC)</t>
-    </r>
+    <t>BTC</t>
   </si>
   <si>
     <t>Date</t>
@@ -59,13 +37,13 @@
     <t>Cost Basis</t>
   </si>
   <si>
-    <t>MakerDao (MKR)</t>
+    <t>MKR</t>
   </si>
   <si>
-    <t>Cardano (ADA)</t>
+    <t>ADA</t>
   </si>
   <si>
-    <t>Ethereum (ETH)</t>
+    <t>ETH</t>
   </si>
 </sst>
 </file>
@@ -76,18 +54,19 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -100,7 +79,9 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <b/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -126,26 +107,29 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -385,347 +369,347 @@
       <c r="S1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>44304.0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>2.0851E-4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>56295.86</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D18" si="1">B3*C3</f>
         <v>11.73824977</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <f>SUM(D3:D1000)</f>
         <v>745.06777</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <f>SUMPRODUCT(D3:D1000/E3,C3:C1000*(C3:C1000&gt;0))</f>
         <v>51211.75349</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="W3" s="6"/>
+      <c r="G3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="W3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>44304.0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>2.8226E-4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>55792.72</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <f t="shared" si="1"/>
         <v>15.74805315</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>44305.0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>0.00270223</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>55120.51</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>148.9482957</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="S5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>44305.0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>0.00154617</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>54339.11</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>84.01750171</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="S6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>44306.0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>8.7419E-4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>54000.01</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>47.20626874</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="S7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="S7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>44307.0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>6.4556E-4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>53950.01</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>34.82796846</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>44308.0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>3.7136E-4</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>53588.05</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>19.90045825</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="M9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>44308.0</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>2.7841E-4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>53641.73</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <f t="shared" si="1"/>
         <v>14.93439405</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>44310.0</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>5.9027E-4</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>50317.72</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <f t="shared" si="1"/>
         <v>29.70104058</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>44310.0</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="8">
         <v>5.1124E-4</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
         <v>50317.72</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <f t="shared" si="1"/>
         <v>25.72443117</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>44315.0</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>9.642E-4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>52500.0</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <f t="shared" si="1"/>
         <v>50.6205</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>44320.0</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>9.2132E-4</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>54000.0</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <f t="shared" si="1"/>
         <v>49.75128</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>44320.0</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>4.6305E-4</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>53700.0</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <f t="shared" si="1"/>
         <v>24.865785</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>44329.0</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>7.9962E-4</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>47285.9</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <f t="shared" si="1"/>
         <v>37.81075136</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>44334.0</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>0.00228857</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>43264.8</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <f t="shared" si="1"/>
         <v>99.01452334</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>44335.0</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>0.00125947</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>39904.3</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <f t="shared" si="1"/>
         <v>50.25826872</v>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="8"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49">
-      <c r="B49" s="8"/>
+      <c r="B49" s="9"/>
     </row>
     <row r="55">
-      <c r="B55" s="8"/>
+      <c r="B55" s="9"/>
     </row>
     <row r="56">
-      <c r="B56" s="8"/>
+      <c r="B56" s="9"/>
     </row>
     <row r="62">
-      <c r="B62" s="8"/>
+      <c r="B62" s="9"/>
     </row>
     <row r="63">
-      <c r="B63" s="8"/>
+      <c r="B63" s="9"/>
     </row>
     <row r="69">
-      <c r="B69" s="8"/>
+      <c r="B69" s="9"/>
     </row>
     <row r="70">
-      <c r="B70" s="8"/>
+      <c r="B70" s="9"/>
     </row>
     <row r="76">
-      <c r="B76" s="8"/>
+      <c r="B76" s="9"/>
     </row>
     <row r="77">
-      <c r="B77" s="8"/>
+      <c r="B77" s="9"/>
     </row>
     <row r="83">
-      <c r="B83" s="8"/>
+      <c r="B83" s="9"/>
     </row>
     <row r="84">
-      <c r="B84" s="8"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="90">
-      <c r="B90" s="8"/>
+      <c r="B90" s="9"/>
     </row>
     <row r="91">
-      <c r="B91" s="8"/>
+      <c r="B91" s="9"/>
     </row>
     <row r="97">
-      <c r="B97" s="8"/>
+      <c r="B97" s="9"/>
     </row>
     <row r="98">
-      <c r="B98" s="8"/>
+      <c r="B98" s="9"/>
     </row>
     <row r="104">
-      <c r="B104" s="8"/>
+      <c r="B104" s="9"/>
     </row>
     <row r="105">
-      <c r="B105" s="8"/>
+      <c r="B105" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -743,154 +727,154 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>44308.0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>0.011192</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>4513.1946</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D10" si="1">B3*C3</f>
         <v>50.51167396</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <f>SUMIF(D3:D1000, "&gt;0")</f>
         <v>301.198274</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <f>SUMPRODUCT(D3:D1000/E3, C3:C1000*(C3:C1000&gt;0))</f>
         <v>3960.337749</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>44308.0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>0.011756</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>4300.0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <f t="shared" si="1"/>
         <v>50.5508</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>44313.0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>0.02294</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>-4500.0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>-103.23</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>44314.0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>0.011709</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>4250.0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>49.76325</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>44315.0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>0.01199</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>4150.0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>49.7585</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>44340.0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>0.023699</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="1">
         <v>-4300.0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>-101.9057</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>44344.0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>0.015286</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>3300.0</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>50.4438</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>44344.0</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>0.015437</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>3250.0</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <f t="shared" si="1"/>
         <v>50.17025</v>
       </c>
@@ -911,139 +895,139 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>44306.0</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="1">
         <v>41.63</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="1">
         <v>1.1364</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D9" si="1">B3*C3</f>
         <v>47.308332</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <f>SUMIF(D3:D1000, "&gt;0")</f>
         <v>157.780619</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <f>SUMPRODUCT(D3:D1000/E3,C3:C1000*(C3:C1000&gt;0))</f>
         <v>1.485416033</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>44312.0</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="1">
         <v>41.63</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="1">
         <v>-1.16</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <f t="shared" si="1"/>
         <v>-48.2908</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>44312.0</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="1">
         <v>20.42</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="1">
         <v>1.1711</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>23.913862</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>44312.0</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="1">
         <v>20.42</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="1">
         <v>-1.18</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>-24.0956</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>44322.0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>15.32</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1.6244</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>24.885808</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>44330.0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>5.5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>2.1686</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>11.9273</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>44335.0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>28.67</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>1.7351</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>49.745317</v>
       </c>
@@ -1064,139 +1048,139 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>44304.0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>0.00178734</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>2189.36</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D9" si="1">B3*C3</f>
         <v>3.913130702</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <f>SUM(D3:D1000)</f>
         <v>338.9823458</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <f>SUMPRODUCT(D3:D1000/E3,C3:C1000*(C3:C1000&gt;0))</f>
         <v>2235.759572</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>44304.0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>0.0073098</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>2157.02</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <f t="shared" si="1"/>
         <v>15.7673848</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>44305.0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>0.05243463</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>2136.44</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>112.0234409</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>44306.0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>2.6755E-4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>2089.16</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>0.558954758</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>44306.0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>0.02988881</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>2089.16</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>62.4425063</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>44306.0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>0.04564034</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>2071.1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>94.52570817</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>44335.0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>0.01665876</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>2986.49</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>49.75122015</v>
       </c>

</xml_diff>

<commit_message>
Updated cost basis logic for sells; fixed test path for CostBasisCalculatorTest
</commit_message>
<xml_diff>
--- a/src/main/resources/Crypto Tracker.xlsx
+++ b/src/main/resources/Crypto Tracker.xlsx
@@ -930,7 +930,7 @@
         <v>1.1364</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D9" si="1">B3*C3</f>
+        <f t="shared" ref="D3:D10" si="1">B3*C3</f>
         <v>47.308332</v>
       </c>
       <c r="E3" s="6">
@@ -1030,6 +1030,21 @@
       <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>49.745317</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>44349.0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>49.49</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-1.8</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="1"/>
+        <v>-89.082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>